<commit_message>
Added access point data export to Excel
</commit_message>
<xml_diff>
--- a/Meraki_Data.xlsx
+++ b/Meraki_Data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,6 +427,11 @@
           <t>Device Name</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Uptime Percentage</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -746,6 +751,256 @@
       </c>
       <c r="B33" t="n">
         <v>100</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>AP-TY-01</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>62.31</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>AP-TY-02</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>61.94</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>AB-1ST-AP-01</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>AB-1ST-AP-05</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>AB-1ST-AP-03</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>AB-1ST-AP-02</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>AB-1ST-AP-04</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>AP-TYEXP-01</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>AP-TYEXP-02</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>DEN-4TH-AP-04</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>62.31</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>DEN-4TH-AP-10</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>62.31</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>AP-TRAVEL</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>DEN-H2W-AP-01</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>62.3</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>DEN-RESPECT-AP</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>62.31</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>DEN-2ND-AP-12</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>62.31</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>RS-AP-01</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>62.31</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>DEN-2ND-AP-03</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>62.3</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>DEN-2ND-AP-06</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>62.3</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>DEN-SIGMA-AP</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>62.3</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>DEN-CREATIVE-AP</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>62.31</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>DEN-TECHNOLOGY-AP</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>62.3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>DEN-SITUATION-AP</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>62.31</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>DEN-2ND-AP-11</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>62.31</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>DEN-4TH-AP-09</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>62.32</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>DEN-EPSILON-AP</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>62.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added initial fresh service request
</commit_message>
<xml_diff>
--- a/Meraki_Data.xlsx
+++ b/Meraki_Data.xlsx
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>100</v>
+        <v>99.98</v>
       </c>
     </row>
     <row r="13">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>100</v>
+        <v>99.97</v>
       </c>
     </row>
     <row r="15">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>100</v>
+        <v>99.97</v>
       </c>
     </row>
     <row r="17">
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
     </row>
     <row r="21">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>100</v>
+        <v>99.97</v>
       </c>
     </row>
     <row r="32">
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>62.31</v>
+        <v>62.32</v>
       </c>
     </row>
     <row r="36">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>61.94</v>
+        <v>62.13</v>
       </c>
     </row>
     <row r="37">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>62.31</v>
+        <v>62.32</v>
       </c>
     </row>
     <row r="45">
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>100</v>
+        <v>99.95</v>
       </c>
     </row>
     <row r="47">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>62.3</v>
+        <v>62.32</v>
       </c>
     </row>
     <row r="48">
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>62.31</v>
+        <v>62.32</v>
       </c>
     </row>
     <row r="49">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>62.31</v>
+        <v>62.32</v>
       </c>
     </row>
     <row r="51">
@@ -930,7 +930,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>62.3</v>
+        <v>62.31</v>
       </c>
     </row>
     <row r="53">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>62.3</v>
+        <v>62.31</v>
       </c>
     </row>
     <row r="56">
@@ -980,7 +980,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>62.31</v>
+        <v>62.3</v>
       </c>
     </row>
     <row r="58">
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>62.32</v>
+        <v>62.31</v>
       </c>
     </row>
     <row r="59">
@@ -1000,7 +1000,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>62.29</v>
+        <v>62.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reformatted the Meraki data to match the desired excel format
</commit_message>
<xml_diff>
--- a/Meraki_Data.xlsx
+++ b/Meraki_Data.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Meraki Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Meraki Switches" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Meraki AP" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,12 +425,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Device Name</t>
+          <t>Switches</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Uptime Percentage</t>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Uptime</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Status</t>
         </is>
       </c>
     </row>
@@ -439,8 +450,18 @@
           <t>DEN-LISTENING</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>100</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>99.91</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -449,8 +470,18 @@
           <t>DEN-RESPECT</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>100</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>99.92</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -459,8 +490,18 @@
           <t>DEN-CREATIVE</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>100</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>99.92</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -469,8 +510,18 @@
           <t>DEN-TECHNOLOGY</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>100</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>99.91</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -479,8 +530,18 @@
           <t>DEN-SIGMA</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>100</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>99.92</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -489,8 +550,18 @@
           <t>DEN-DIST-02</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>100</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -499,8 +570,18 @@
           <t>DEN-DIST-01</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>100</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -509,8 +590,18 @@
           <t>DEN-2ND-03-F</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>100</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>100</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -519,8 +610,18 @@
           <t>DEN-2ND-05-H</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>100</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -529,8 +630,18 @@
           <t>DEN-2ND-02-E</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>100</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -539,8 +650,18 @@
           <t>DEN-2ND-01-D</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
         <v>99.98</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -549,8 +670,18 @@
           <t>DEN-2ND-06-I</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>100</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>100</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -559,8 +690,18 @@
           <t>DEN-2ND-04-G</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
         <v>99.97</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -569,8 +710,18 @@
           <t>DEN-4TH-SOUTH</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>100</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>100</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -579,8 +730,18 @@
           <t>DEN-2ND-07-J</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
         <v>99.97</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -589,8 +750,18 @@
           <t>DEN-2ND-08-K</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>100</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>100</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -599,8 +770,18 @@
           <t>DEN-H2W</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>100</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>100</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -609,8 +790,18 @@
           <t>DEN-CORE-01</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>100</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>100</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -619,8 +810,18 @@
           <t>DEN-CORE-02</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
         <v>99.98999999999999</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -629,8 +830,18 @@
           <t>TY-S200-01</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>100</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>TYLER</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>100</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -639,8 +850,18 @@
           <t>TY-S100-01</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>100</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>TYLER</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>100</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -649,8 +870,18 @@
           <t>AB-1ST-03</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>100</v>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ABILENE</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>100</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -659,8 +890,18 @@
           <t>AB-1ST-01</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>100</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ABILENE</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>100</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -669,8 +910,18 @@
           <t>DEN-4TH-03-C</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>100</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>100</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -679,8 +930,18 @@
           <t>AB-1ST-02</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>100</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ABILENE</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>100</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -689,8 +950,18 @@
           <t>TY-EXP-1</t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>100</v>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>TYLER</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>100</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -699,8 +970,18 @@
           <t>DEN-4TH-02-B</t>
         </is>
       </c>
-      <c r="B28" t="n">
-        <v>100</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>100</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -709,8 +990,18 @@
           <t>DEN-4TH-01-A</t>
         </is>
       </c>
-      <c r="B29" t="n">
-        <v>100</v>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>100</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -719,8 +1010,18 @@
           <t>DEN-1ST-TEMP</t>
         </is>
       </c>
-      <c r="B30" t="n">
-        <v>100</v>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>100</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -729,8 +1030,18 @@
           <t>RS-2ND-01-A</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ROCK SPRINGS</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
         <v>99.97</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -739,8 +1050,18 @@
           <t>DEN-ISP-01</t>
         </is>
       </c>
-      <c r="B32" t="n">
-        <v>100</v>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>100</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -749,258 +1070,559 @@
           <t>DEN-EPSILON</t>
         </is>
       </c>
-      <c r="B33" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>99.91</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Access Points</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Uptime</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>AP-TY-01</t>
         </is>
       </c>
-      <c r="B35" t="n">
-        <v>62.32</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TYLER</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>67.03</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>AP-TY-02</t>
         </is>
       </c>
-      <c r="B36" t="n">
-        <v>62.13</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TYLER</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>66.8</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>AB-1ST-AP-01</t>
         </is>
       </c>
-      <c r="B37" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ABILENE</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>AB-1ST-AP-05</t>
         </is>
       </c>
-      <c r="B38" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ABILENE</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>AB-1ST-AP-03</t>
         </is>
       </c>
-      <c r="B39" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ABILENE</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>AB-1ST-AP-02</t>
         </is>
       </c>
-      <c r="B40" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ABILENE</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>AB-1ST-AP-04</t>
         </is>
       </c>
-      <c r="B41" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ABILENE</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>AP-TYEXP-01</t>
         </is>
       </c>
-      <c r="B42" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>TYLER</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>100</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>AP-TYEXP-02</t>
         </is>
       </c>
-      <c r="B43" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TYLER</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
         <is>
           <t>DEN-4TH-AP-04</t>
         </is>
       </c>
-      <c r="B44" t="n">
-        <v>62.32</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>67.63</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
         <is>
           <t>DEN-4TH-AP-10</t>
         </is>
       </c>
-      <c r="B45" t="n">
-        <v>62.31</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>67.61</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
         <is>
           <t>AP-TRAVEL</t>
         </is>
       </c>
-      <c r="B46" t="n">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
         <v>99.95</v>
       </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>DEN-H2W-AP-01</t>
         </is>
       </c>
-      <c r="B47" t="n">
-        <v>62.32</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>67.61</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>DEN-RESPECT-AP</t>
         </is>
       </c>
-      <c r="B48" t="n">
-        <v>62.32</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>67.51000000000001</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
         <is>
           <t>DEN-2ND-AP-12</t>
         </is>
       </c>
-      <c r="B49" t="n">
-        <v>62.31</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>67.61</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>RS-AP-01</t>
         </is>
       </c>
-      <c r="B50" t="n">
-        <v>62.32</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ROCK SPRINGS</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>67.61</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
         <is>
           <t>DEN-2ND-AP-03</t>
         </is>
       </c>
-      <c r="B51" t="n">
-        <v>62.3</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>67.62</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
         <is>
           <t>DEN-2ND-AP-06</t>
         </is>
       </c>
-      <c r="B52" t="n">
-        <v>62.31</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>67.62</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
         <is>
           <t>DEN-SIGMA-AP</t>
         </is>
       </c>
-      <c r="B53" t="n">
-        <v>62.3</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>67.61</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
         <is>
           <t>DEN-CREATIVE-AP</t>
         </is>
       </c>
-      <c r="B54" t="n">
-        <v>62.31</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
         <is>
           <t>DEN-TECHNOLOGY-AP</t>
         </is>
       </c>
-      <c r="B55" t="n">
-        <v>62.31</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>67.51000000000001</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
         <is>
           <t>DEN-SITUATION-AP</t>
         </is>
       </c>
-      <c r="B56" t="n">
-        <v>62.31</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>67.61</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
         <is>
           <t>DEN-2ND-AP-11</t>
         </is>
       </c>
-      <c r="B57" t="n">
-        <v>62.3</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>67.61</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
         <is>
           <t>DEN-4TH-AP-09</t>
         </is>
       </c>
-      <c r="B58" t="n">
-        <v>62.31</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>67.61</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
         <is>
           <t>DEN-EPSILON-AP</t>
         </is>
       </c>
-      <c r="B59" t="n">
-        <v>62.3</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>DENVER</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>67.61</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>offline</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got freshservice requests working with query filters
</commit_message>
<xml_diff>
--- a/Meraki_Data.xlsx
+++ b/Meraki_Data.xlsx
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>99.98</v>
+        <v>100</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -696,7 +696,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>99.97</v>
+        <v>100</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>99.97</v>
+        <v>100</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -816,7 +816,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>99.98999999999999</v>
+        <v>100</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1036,7 +1036,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>99.97</v>
+        <v>100</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1137,11 +1137,11 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>66.95999999999999</v>
+        <v>62.31</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1157,11 +1157,11 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>66.73</v>
+        <v>61.96</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1317,11 +1317,11 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>67.55</v>
+        <v>62.31</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1337,11 +1337,11 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>67.54000000000001</v>
+        <v>62.3</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>99.95</v>
+        <v>100</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1377,11 +1377,11 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>67.54000000000001</v>
+        <v>62.29</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1397,11 +1397,11 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>67.44</v>
+        <v>62.19</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1417,11 +1417,11 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>67.54000000000001</v>
+        <v>62.29</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1437,11 +1437,11 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>67.53</v>
+        <v>62.29</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1457,11 +1457,11 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>67.54000000000001</v>
+        <v>62.3</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1477,11 +1477,11 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>67.55</v>
+        <v>62.31</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1497,11 +1497,11 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>67.54000000000001</v>
+        <v>62.3</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1517,11 +1517,11 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>67.43000000000001</v>
+        <v>62.19</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1537,11 +1537,11 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>67.44</v>
+        <v>62.2</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1557,11 +1557,11 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>67.54000000000001</v>
+        <v>62.3</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1577,11 +1577,11 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>67.54000000000001</v>
+        <v>62.3</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1597,11 +1597,11 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>67.54000000000001</v>
+        <v>62.3</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>
@@ -1617,11 +1617,11 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>67.54000000000001</v>
+        <v>62.3</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed fresh service data retrieval and export to excel
</commit_message>
<xml_diff>
--- a/Meraki_Data.xlsx
+++ b/Meraki_Data.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Meraki Switches" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Meraki AP" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Freshservice" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1137,11 +1138,11 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>62.31</v>
+        <v>66.84</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1157,11 +1158,11 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>61.96</v>
+        <v>66.48999999999999</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1317,11 +1318,11 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>62.31</v>
+        <v>67.44</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1337,11 +1338,11 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>62.3</v>
+        <v>67.43000000000001</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1377,11 +1378,11 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>62.29</v>
+        <v>67.43000000000001</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1397,11 +1398,11 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>62.19</v>
+        <v>67.33</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1417,11 +1418,11 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>62.29</v>
+        <v>67.43000000000001</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1437,11 +1438,11 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>62.29</v>
+        <v>67.44</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1457,11 +1458,11 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>62.3</v>
+        <v>67.44</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1477,11 +1478,11 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>62.31</v>
+        <v>67.44</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1497,11 +1498,11 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>62.3</v>
+        <v>67.44</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1517,11 +1518,11 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>62.19</v>
+        <v>67.33</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1537,11 +1538,11 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>62.2</v>
+        <v>67.33</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1557,11 +1558,11 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>62.3</v>
+        <v>67.43000000000001</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1577,11 +1578,11 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>62.3</v>
+        <v>67.44</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1597,11 +1598,11 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>62.3</v>
+        <v>67.43000000000001</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>offline</t>
         </is>
       </c>
     </row>
@@ -1617,12 +1618,59 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>62.3</v>
+        <v>67.44</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>online</t>
-        </is>
+          <t>offline</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Total Tickets (Last 7 Days)</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Unresolved Tickets (Last 7 Days)</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Resolved Tickets (Last 7 Days)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>